<commit_message>
add MBs to file size label
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/hrs_ccd_case_definition.xlsx
+++ b/src/functionalTest/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -438,7 +438,7 @@
     <t xml:space="preserve">Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Hearing File Size</t>
+    <t xml:space="preserve">Hearing File Size (MBs)</t>
   </si>
   <si>
     <t xml:space="preserve">File size in MBs</t>
@@ -9514,8 +9514,8 @@
   </sheetPr>
   <dimension ref="A1:IU18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10458,7 +10458,7 @@
   </sheetPr>
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L37" activeCellId="0" sqref="L37"/>
     </sheetView>
   </sheetViews>

</xml_diff>